<commit_message>
Updated category for software `lumpy` in file `CLCA_container_info.xlsx`
</commit_message>
<xml_diff>
--- a/container/CLCA_container_info.xlsx
+++ b/container/CLCA_container_info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rpackage\CLCA_WGS\container\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -924,10 +924,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>

</xml_diff>